<commit_message>
edit code section and admin permission
</commit_message>
<xml_diff>
--- a/public/assets/templates/excels/customers-list.xlsx
+++ b/public/assets/templates/excels/customers-list.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Worksheet'!$A$2:$F$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Worksheet'!$A$2:$F$13</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>Danh sách khách hàng</t>
   </si>
@@ -58,9 +58,24 @@
     <t>125, CIT, Đại học Cần Thơ</t>
   </si>
   <si>
+    <t>VN</t>
+  </si>
+  <si>
     <t>Nguyễn Văn Lý</t>
   </si>
   <si>
+    <t>Nguyễn VăHoàng</t>
+  </si>
+  <si>
+    <t>aduy644@gmail.com</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Hoàng</t>
+  </si>
+  <si>
+    <t>Nguyễn Duy Anh</t>
+  </si>
+  <si>
     <t>Nguyen Van Minh Sau Hai</t>
   </si>
   <si>
@@ -71,6 +86,9 @@
   </si>
   <si>
     <t>ndanhdev5@gmail.com</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Tài</t>
   </si>
   <si>
     <t>Nguyễn Văn Tân</t>
@@ -460,10 +478,10 @@
   <sheetPr filterMode="1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A8" sqref="A8:F8"/>
+      <selection activeCell="A13" sqref="A13:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -544,10 +562,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
@@ -556,15 +574,15 @@
         <v>10</v>
       </c>
       <c r="E5" s="3">
-        <v>2000</v>
+        <v>1989</v>
       </c>
       <c r="F5" s="3">
-        <v>3625257456</v>
+        <v>123456789</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
@@ -584,36 +602,36 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E7" s="3">
-        <v>2001</v>
+        <v>1989</v>
       </c>
       <c r="F7" s="3">
-        <v>362525745</v>
+        <v>123456789</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E8" s="4">
         <v>1989</v>
@@ -623,10 +641,110 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="F9"/>
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1989</v>
+      </c>
+      <c r="F9" s="3">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2000</v>
+      </c>
+      <c r="F10" s="4">
+        <v>3625257456</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2001</v>
+      </c>
+      <c r="F11" s="3">
+        <v>362525745</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1989</v>
+      </c>
+      <c r="F12" s="4">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1989</v>
+      </c>
+      <c r="F13" s="3">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="F14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:F8"/>
+  <autoFilter ref="A2:F13"/>
   <mergeCells>
     <mergeCell ref="A1:F1"/>
   </mergeCells>

</xml_diff>